<commit_message>
Object detection code 9
Added comments
</commit_message>
<xml_diff>
--- a/OSPAR_Test.xlsx
+++ b/OSPAR_Test.xlsx
@@ -478,4 +478,279 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007728B73E428748448E0B2E963AA8FA9C" ma:contentTypeVersion="16" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="83942090f8152eb43b423cb5024201fe">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fa7938fd-c11d-453b-9a6d-4a84f56bdf9a" xmlns:ns3="79231145-eb60-443c-99fd-e6924c3bf250" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86d9ca6f310037a55b812eedba8da2db" ns2:_="" ns3:_="">
+    <xsd:import namespace="fa7938fd-c11d-453b-9a6d-4a84f56bdf9a"/>
+    <xsd:import namespace="79231145-eb60-443c-99fd-e6924c3bf250"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fa7938fd-c11d-453b-9a6d-4a84f56bdf9a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Afbeeldingtags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="03a34951-496f-4c01-b4ba-4cbd104b361e" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="79231145-eb60-443c-99fd-e6924c3bf250" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Gedeeld met" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Gedeeld met details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{a742754f-4457-45f7-acf7-394694d75e3b}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="79231145-eb60-443c-99fd-e6924c3bf250">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhoudstype"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fa7938fd-c11d-453b-9a6d-4a84f56bdf9a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="79231145-eb60-443c-99fd-e6924c3bf250" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2C0CB8-33B4-4DCF-B566-6665A35B862E}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78BC2F5E-E606-410B-977F-7CC36611273A}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C51F16D8-E993-419B-84BF-BC778E2E0E94}"/>
 </file>
</xml_diff>

<commit_message>
New model, new line
</commit_message>
<xml_diff>
--- a/OSPAR_Test.xlsx
+++ b/OSPAR_Test.xlsx
@@ -9,6 +9,10 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -672,6 +676,342 @@
       <c r="B3" t="n">
         <v>0</v>
       </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Plastic folies of stukken daarvan 2.5 - 50 cm</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Snoep snack en chips verpakkingen</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Voedselverpakkingen</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Sheet number</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Drankblikjes</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Drankflessen &lt; 1/2 liter</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Plastic folies of stukken daarvan 2.5 - 50 cm</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Snoep snack en chips verpakkingen</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Voedselverpakkingen</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Sheet number</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Drankblikjes</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Drankflessen &lt; 1/2 liter</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Plastic folies of stukken daarvan 2.5 - 50 cm</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Snoep snack en chips verpakkingen</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Voedselverpakkingen</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Sheet number</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Drankblikjes</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Drankflessen &lt; 1/2 liter</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Plastic folies of stukken daarvan 2.5 - 50 cm</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Snoep snack en chips verpakkingen</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Voedselverpakkingen</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Sheet number</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Drankblikjes</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Drankflessen &lt; 1/2 liter</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
       <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -965,9 +1305,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92A54130-6B00-4B73-B94F-2C229EC52AA9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{619CDB02-4414-4EC2-A0D3-AB9C2BF05F9E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80270E86-BC8E-4E27-AF11-DEFA394D238A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D694040B-2036-4F0C-A70C-BFBAFD19E3B8}"/>
 </file>
</xml_diff>